<commit_message>
updated external + element + hid pycache folders
</commit_message>
<xml_diff>
--- a/post_processing/Relationships.xlsx
+++ b/post_processing/Relationships.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mordrel-my.sharepoint.com/personal/matthieu_mordrel_pro/Documents/Work/Projects/Kovera/Project 2/Scripts/Project/post_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_4EF780B4CC196D1A09DC4B1F3E8DCC8FF1D1DF0B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAB6B4CD-7236-46D4-8A3E-515C5856D4E9}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_4EF780B4CC196D1A09DC4B1F3E8DCC8FF1D1DF0B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87D39218-A16F-4F07-A558-8B4DB55682F7}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="3510" windowWidth="29040" windowHeight="15840" tabRatio="693" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1357,10 +1357,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1629,7 +1625,7 @@
   <dimension ref="A1:E336"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="A3" sqref="A3:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,7 +1662,7 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="E3" t="str">
+      <c r="E3" t="str" cm="1">
         <f t="array" ref="E3:E209">_xlfn.UNIQUE(_xlfn.VSTACK(A3:A31,A36:A336))</f>
         <v>CKPL213F88_1</v>
       </c>
@@ -5938,7 +5934,7 @@
   <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>